<commit_message>
hotfix: fix the bug with docs directory.
</commit_message>
<xml_diff>
--- a/docs/feedback.xlsx
+++ b/docs/feedback.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\TAs_automate\Group_Presentation\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\GitHub\auto-feedbacker\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69A654DA-4A71-4ABD-9D2C-A155C996FFCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{127D8476-ACAF-42CA-AAA8-D92667DEB17F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2565" yWindow="3000" windowWidth="21600" windowHeight="11265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -420,7 +420,7 @@
   <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -522,7 +522,7 @@
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
-      <c r="H8" s="1"/>
+      <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
@@ -542,7 +542,7 @@
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
-      <c r="H10" s="2"/>
+      <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
@@ -562,7 +562,7 @@
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
-      <c r="H12" s="2"/>
+      <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
@@ -572,7 +572,7 @@
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
-      <c r="H13" s="1"/>
+      <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
@@ -592,7 +592,7 @@
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
-      <c r="H15" s="1"/>
+      <c r="H15" s="2"/>
     </row>
     <row r="16" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
@@ -652,7 +652,7 @@
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
-      <c r="H21" s="1"/>
+      <c r="H21" s="2"/>
     </row>
     <row r="22" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
@@ -662,7 +662,7 @@
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
-      <c r="H22" s="2"/>
+      <c r="H22" s="1"/>
     </row>
     <row r="23" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
@@ -732,7 +732,7 @@
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
-      <c r="H29" s="2"/>
+      <c r="H29" s="1"/>
     </row>
     <row r="30" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
@@ -742,7 +742,7 @@
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
-      <c r="H30" s="1"/>
+      <c r="H30" s="2"/>
     </row>
     <row r="31" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
@@ -752,7 +752,7 @@
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
-      <c r="H31" s="2"/>
+      <c r="H31" s="1"/>
     </row>
     <row r="32" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
@@ -762,7 +762,7 @@
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
-      <c r="H32" s="2"/>
+      <c r="H32" s="1"/>
     </row>
     <row r="33" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
@@ -772,7 +772,7 @@
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
-      <c r="H33" s="2"/>
+      <c r="H33" s="1"/>
     </row>
     <row r="34" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3"/>
@@ -782,7 +782,7 @@
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
-      <c r="H34" s="2"/>
+      <c r="H34" s="1"/>
     </row>
     <row r="35" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3"/>
@@ -792,7 +792,7 @@
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
-      <c r="H35" s="1"/>
+      <c r="H35" s="2"/>
     </row>
     <row r="36" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
@@ -802,7 +802,7 @@
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
-      <c r="H36" s="2"/>
+      <c r="H36" s="1"/>
     </row>
     <row r="37" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
@@ -812,7 +812,7 @@
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
-      <c r="H37" s="1"/>
+      <c r="H37" s="2"/>
     </row>
     <row r="38" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3"/>
@@ -822,7 +822,7 @@
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
-      <c r="H38" s="2"/>
+      <c r="H38" s="1"/>
     </row>
     <row r="39" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="3"/>
@@ -832,7 +832,7 @@
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
-      <c r="H39" s="1"/>
+      <c r="H39" s="2"/>
     </row>
     <row r="40" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="3"/>

</xml_diff>

<commit_message>
feat: add peer evaluation mode
</commit_message>
<xml_diff>
--- a/docs/feedback.xlsx
+++ b/docs/feedback.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\GitHub\auto-feedbacker\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{127D8476-ACAF-42CA-AAA8-D92667DEB17F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D05E9925-089D-41AE-82CE-26CB9CDD4556}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2565" yWindow="3000" windowWidth="21600" windowHeight="11265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -417,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
+      <selection activeCell="L61" sqref="L61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -522,7 +522,7 @@
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
-      <c r="H8" s="2"/>
+      <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
@@ -542,7 +542,7 @@
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
-      <c r="H10" s="1"/>
+      <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
@@ -562,7 +562,7 @@
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
-      <c r="H12" s="1"/>
+      <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
@@ -572,7 +572,7 @@
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
-      <c r="H13" s="2"/>
+      <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
@@ -592,7 +592,7 @@
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
-      <c r="H15" s="2"/>
+      <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
@@ -652,7 +652,7 @@
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
-      <c r="H21" s="2"/>
+      <c r="H21" s="1"/>
     </row>
     <row r="22" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
@@ -662,7 +662,7 @@
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
-      <c r="H22" s="1"/>
+      <c r="H22" s="2"/>
     </row>
     <row r="23" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
@@ -732,7 +732,7 @@
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
-      <c r="H29" s="1"/>
+      <c r="H29" s="2"/>
     </row>
     <row r="30" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
@@ -742,7 +742,7 @@
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
-      <c r="H30" s="2"/>
+      <c r="H30" s="1"/>
     </row>
     <row r="31" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
@@ -752,7 +752,7 @@
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
-      <c r="H31" s="1"/>
+      <c r="H31" s="2"/>
     </row>
     <row r="32" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
@@ -762,7 +762,7 @@
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
-      <c r="H32" s="1"/>
+      <c r="H32" s="2"/>
     </row>
     <row r="33" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
@@ -772,7 +772,7 @@
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
-      <c r="H33" s="1"/>
+      <c r="H33" s="2"/>
     </row>
     <row r="34" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3"/>
@@ -782,7 +782,7 @@
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
-      <c r="H34" s="1"/>
+      <c r="H34" s="2"/>
     </row>
     <row r="35" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3"/>
@@ -792,7 +792,7 @@
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
-      <c r="H35" s="2"/>
+      <c r="H35" s="1"/>
     </row>
     <row r="36" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
@@ -802,7 +802,7 @@
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
-      <c r="H36" s="1"/>
+      <c r="H36" s="2"/>
     </row>
     <row r="37" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
@@ -812,7 +812,7 @@
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
-      <c r="H37" s="2"/>
+      <c r="H37" s="1"/>
     </row>
     <row r="38" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3"/>
@@ -822,7 +822,7 @@
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
-      <c r="H38" s="1"/>
+      <c r="H38" s="2"/>
     </row>
     <row r="39" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="3"/>
@@ -832,7 +832,7 @@
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
-      <c r="H39" s="2"/>
+      <c r="H39" s="1"/>
     </row>
     <row r="40" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="3"/>
@@ -854,6 +854,26 @@
       <c r="G41" s="3"/>
       <c r="H41" s="2"/>
     </row>
+    <row r="42" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="3"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="1"/>
+    </row>
+    <row r="43" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="3"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="1"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>